<commit_message>
Fix in Inbevec's template
</commit_message>
<xml_diff>
--- a/Projects/INBEVEC/Data/Template.xlsx
+++ b/Projects/INBEVEC/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Relative Positioning" sheetId="1" state="visible" r:id="rId2"/>
@@ -338,25 +338,25 @@
     <t xml:space="preserve">BUDWEISER At Equipo de frio – Disponibilidad</t>
   </si>
   <si>
-    <t xml:space="preserve">BUDWEISER</t>
+    <t xml:space="preserve">Budweiser</t>
   </si>
   <si>
     <t xml:space="preserve">PILSENER LIGHT At Equipo de frio – Disponibilidad</t>
   </si>
   <si>
-    <t xml:space="preserve">PILSENER LIGHT</t>
+    <t xml:space="preserve">Pilsener Light</t>
   </si>
   <si>
     <t xml:space="preserve">CLUB PREMIUM At Equipo de frio – Disponibilidad</t>
   </si>
   <si>
-    <t xml:space="preserve">CLUB PREMIUM</t>
+    <t xml:space="preserve">Club Premium</t>
   </si>
   <si>
     <t xml:space="preserve">PILSENER At Equipo de frio – Disponibilidad</t>
   </si>
   <si>
-    <t xml:space="preserve">PILSENER</t>
+    <t xml:space="preserve">Pilsener</t>
   </si>
   <si>
     <t xml:space="preserve">PONY MALTA At Equipo de frio – Disponibilidad</t>
@@ -836,23 +836,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.4251012145749"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.9757085020243"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="56.4372469635627"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.9514170040486"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.6437246963563"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.4898785425101"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.6437246963563"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.4251012145749"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.9959514170041"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.3036437246964"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="17.6234817813765"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.0404858299595"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.9554655870445"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="30.1133603238866"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="9.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.78947368421053"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.834008097166"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.5991902834008"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.2793522267206"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.1174089068826"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.82995951417"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.1174089068826"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.78947368421053"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.7327935222672"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.8744939271255"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="22.6437246963563"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="18.7327935222672"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.0526315789474"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="20.3238866396761"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="32.3198380566802"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="9.78947368421053"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1537,64 +1537,64 @@
   </sheetPr>
   <dimension ref="B1:F14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.18623481781377"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.0121457489879"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.0121457489879"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.1133603238866"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.2995951417004"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.7044534412955"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.66801619433198"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="39.663967611336"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.3684210526316"/>
-    <col collapsed="false" hidden="false" max="253" min="10" style="0" width="8.81376518218623"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.0769230769231"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.5587044534413"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.3198380566802"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.3967611336032"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.0404858299595"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="42.4817813765182"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="253" min="10" style="0" width="9.30364372469636"/>
     <col collapsed="false" hidden="false" max="254" min="254" style="0" width="3.18623481781377"/>
-    <col collapsed="false" hidden="false" max="255" min="255" style="0" width="20.3238866396761"/>
-    <col collapsed="false" hidden="false" max="256" min="256" style="0" width="79.5748987854251"/>
+    <col collapsed="false" hidden="false" max="255" min="255" style="0" width="21.5465587044534"/>
+    <col collapsed="false" hidden="false" max="256" min="256" style="0" width="85.5748987854251"/>
     <col collapsed="false" hidden="false" max="257" min="257" style="0" width="3.42914979757085"/>
-    <col collapsed="false" hidden="false" max="258" min="258" style="0" width="14.0769230769231"/>
-    <col collapsed="false" hidden="false" max="259" min="259" style="0" width="30.1133603238866"/>
-    <col collapsed="false" hidden="false" max="260" min="260" style="0" width="42.2348178137652"/>
-    <col collapsed="false" hidden="false" max="261" min="261" style="0" width="15.7975708502024"/>
-    <col collapsed="false" hidden="false" max="262" min="262" style="0" width="6.61133603238866"/>
-    <col collapsed="false" hidden="false" max="263" min="263" style="0" width="9.66801619433198"/>
-    <col collapsed="false" hidden="false" max="264" min="264" style="0" width="39.663967611336"/>
-    <col collapsed="false" hidden="false" max="265" min="265" style="0" width="18.3684210526316"/>
-    <col collapsed="false" hidden="false" max="509" min="266" style="0" width="8.81376518218623"/>
+    <col collapsed="false" hidden="false" max="258" min="258" style="0" width="15.0526315789474"/>
+    <col collapsed="false" hidden="false" max="259" min="259" style="0" width="32.3198380566802"/>
+    <col collapsed="false" hidden="false" max="260" min="260" style="0" width="45.417004048583"/>
+    <col collapsed="false" hidden="false" max="261" min="261" style="0" width="16.7732793522267"/>
+    <col collapsed="false" hidden="false" max="262" min="262" style="0" width="6.97570850202429"/>
+    <col collapsed="false" hidden="false" max="263" min="263" style="0" width="10.0404858299595"/>
+    <col collapsed="false" hidden="false" max="264" min="264" style="0" width="42.4817813765182"/>
+    <col collapsed="false" hidden="false" max="265" min="265" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="509" min="266" style="0" width="9.30364372469636"/>
     <col collapsed="false" hidden="false" max="510" min="510" style="0" width="3.18623481781377"/>
-    <col collapsed="false" hidden="false" max="511" min="511" style="0" width="20.3238866396761"/>
-    <col collapsed="false" hidden="false" max="512" min="512" style="0" width="79.5748987854251"/>
+    <col collapsed="false" hidden="false" max="511" min="511" style="0" width="21.5465587044534"/>
+    <col collapsed="false" hidden="false" max="512" min="512" style="0" width="85.5748987854251"/>
     <col collapsed="false" hidden="false" max="513" min="513" style="0" width="3.42914979757085"/>
-    <col collapsed="false" hidden="false" max="514" min="514" style="0" width="14.0769230769231"/>
-    <col collapsed="false" hidden="false" max="515" min="515" style="0" width="30.1133603238866"/>
-    <col collapsed="false" hidden="false" max="516" min="516" style="0" width="42.2348178137652"/>
-    <col collapsed="false" hidden="false" max="517" min="517" style="0" width="15.7975708502024"/>
-    <col collapsed="false" hidden="false" max="518" min="518" style="0" width="6.61133603238866"/>
-    <col collapsed="false" hidden="false" max="519" min="519" style="0" width="9.66801619433198"/>
-    <col collapsed="false" hidden="false" max="520" min="520" style="0" width="39.663967611336"/>
-    <col collapsed="false" hidden="false" max="521" min="521" style="0" width="18.3684210526316"/>
-    <col collapsed="false" hidden="false" max="765" min="522" style="0" width="8.81376518218623"/>
+    <col collapsed="false" hidden="false" max="514" min="514" style="0" width="15.0526315789474"/>
+    <col collapsed="false" hidden="false" max="515" min="515" style="0" width="32.3198380566802"/>
+    <col collapsed="false" hidden="false" max="516" min="516" style="0" width="45.417004048583"/>
+    <col collapsed="false" hidden="false" max="517" min="517" style="0" width="16.7732793522267"/>
+    <col collapsed="false" hidden="false" max="518" min="518" style="0" width="6.97570850202429"/>
+    <col collapsed="false" hidden="false" max="519" min="519" style="0" width="10.0404858299595"/>
+    <col collapsed="false" hidden="false" max="520" min="520" style="0" width="42.4817813765182"/>
+    <col collapsed="false" hidden="false" max="521" min="521" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="765" min="522" style="0" width="9.30364372469636"/>
     <col collapsed="false" hidden="false" max="766" min="766" style="0" width="3.18623481781377"/>
-    <col collapsed="false" hidden="false" max="767" min="767" style="0" width="20.3238866396761"/>
-    <col collapsed="false" hidden="false" max="768" min="768" style="0" width="79.5748987854251"/>
+    <col collapsed="false" hidden="false" max="767" min="767" style="0" width="21.5465587044534"/>
+    <col collapsed="false" hidden="false" max="768" min="768" style="0" width="85.5748987854251"/>
     <col collapsed="false" hidden="false" max="769" min="769" style="0" width="3.42914979757085"/>
-    <col collapsed="false" hidden="false" max="770" min="770" style="0" width="14.0769230769231"/>
-    <col collapsed="false" hidden="false" max="771" min="771" style="0" width="30.1133603238866"/>
-    <col collapsed="false" hidden="false" max="772" min="772" style="0" width="42.2348178137652"/>
-    <col collapsed="false" hidden="false" max="773" min="773" style="0" width="15.7975708502024"/>
-    <col collapsed="false" hidden="false" max="774" min="774" style="0" width="6.61133603238866"/>
-    <col collapsed="false" hidden="false" max="775" min="775" style="0" width="9.66801619433198"/>
-    <col collapsed="false" hidden="false" max="776" min="776" style="0" width="39.663967611336"/>
-    <col collapsed="false" hidden="false" max="777" min="777" style="0" width="18.3684210526316"/>
-    <col collapsed="false" hidden="false" max="1021" min="778" style="0" width="8.81376518218623"/>
+    <col collapsed="false" hidden="false" max="770" min="770" style="0" width="15.0526315789474"/>
+    <col collapsed="false" hidden="false" max="771" min="771" style="0" width="32.3198380566802"/>
+    <col collapsed="false" hidden="false" max="772" min="772" style="0" width="45.417004048583"/>
+    <col collapsed="false" hidden="false" max="773" min="773" style="0" width="16.7732793522267"/>
+    <col collapsed="false" hidden="false" max="774" min="774" style="0" width="6.97570850202429"/>
+    <col collapsed="false" hidden="false" max="775" min="775" style="0" width="10.0404858299595"/>
+    <col collapsed="false" hidden="false" max="776" min="776" style="0" width="42.4817813765182"/>
+    <col collapsed="false" hidden="false" max="777" min="777" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1021" min="778" style="0" width="9.30364372469636"/>
     <col collapsed="false" hidden="false" max="1022" min="1022" style="0" width="3.18623481781377"/>
-    <col collapsed="false" hidden="false" max="1023" min="1023" style="0" width="20.3238866396761"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="79.5748987854251"/>
+    <col collapsed="false" hidden="false" max="1023" min="1023" style="0" width="21.5465587044534"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="85.5748987854251"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1770,17 +1770,17 @@
   <dimension ref="B2:E65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.81376518218623"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.3805668016194"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.8097165991903"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.8947368421053"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.7975708502024"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.81376518218623"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.30364372469636"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.587044534413"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.0364372469636"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.7732793522267"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.30364372469636"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>